<commit_message>
Finalize tables for Jessica
</commit_message>
<xml_diff>
--- a/Tables/Fig13_Table_Fragmentation.xlsx
+++ b/Tables/Fig13_Table_Fragmentation.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="county" r:id="rId3" sheetId="1"/>
+    <sheet name="region" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="44">
   <si>
     <t>county</t>
   </si>
@@ -114,6 +115,36 @@
   </si>
   <si>
     <t>Large Core</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>acres_2013_sum</t>
+  </si>
+  <si>
+    <t>acres_2018_sum</t>
+  </si>
+  <si>
+    <t>acres_change_sum</t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>Lower Eastern</t>
+  </si>
+  <si>
+    <t>North Central</t>
+  </si>
+  <si>
+    <t>Southern</t>
+  </si>
+  <si>
+    <t>Upper Eastern</t>
+  </si>
+  <si>
+    <t>Western</t>
   </si>
 </sst>
 </file>
@@ -2224,4 +2255,544 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.4169916E9</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.3776295E9</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-3.93621E7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3.501707E8</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3.699718E8</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.98011E7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9.23882E7</v>
+      </c>
+      <c r="D4" t="n">
+        <v>9.17631E7</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-625100.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3.77738E7</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3.13358E7</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-6438000.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2.01689E8</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.748417E8</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-2.68473E7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="n">
+        <v>8.579521E8</v>
+      </c>
+      <c r="D7" t="n">
+        <v>8.617905E8</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3838400.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8.03316E7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>7.17352E7</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-8596400.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.527591E8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.806191E8</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2.786E7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="n">
+        <v>9.13762E7</v>
+      </c>
+      <c r="D10" t="n">
+        <v>9.99942E7</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8618000.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2.150541E8</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2.099762E8</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-5077900.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="n">
+        <v>7.650438E8</v>
+      </c>
+      <c r="D12" t="n">
+        <v>7.536915E8</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-1.13523E7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2.270949E8</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2.270017E8</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-93200.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8516800.0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>8509100.0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-7700.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1.071822E8</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.077294E8</v>
+      </c>
+      <c r="E16" t="n">
+        <v>547200.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.0102599E9</v>
+      </c>
+      <c r="D17" t="n">
+        <v>9.983865E8</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-1.18734E7</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="n">
+        <v>9.72534E7</v>
+      </c>
+      <c r="D18" t="n">
+        <v>9.71898E7</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-63600.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="n">
+        <v>8.05034E7</v>
+      </c>
+      <c r="D19" t="n">
+        <v>7.54795E7</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-5023900.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="n">
+        <v>6.58343E7</v>
+      </c>
+      <c r="D20" t="n">
+        <v>7.5516E7</v>
+      </c>
+      <c r="E20" t="n">
+        <v>9681700.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2.262284E8</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2.194885E8</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-6739900.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1.1729172E9</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.1723489E9</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-568300.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1.80669E8</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.806224E8</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-46600.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1.192464E8</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.202824E8</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1036000.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="n">
+        <v>7.49598E7</v>
+      </c>
+      <c r="D25" t="n">
+        <v>6.98902E7</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-5069600.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" t="n">
+        <v>2.577044E8</v>
+      </c>
+      <c r="D26" t="n">
+        <v>2.564097E8</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-1294700.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1.2344886E9</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1.2355982E9</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1109600.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="n">
+        <v>8.21802E7</v>
+      </c>
+      <c r="D28" t="n">
+        <v>8.42515E7</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2071300.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="n">
+        <v>8.988549E8</v>
+      </c>
+      <c r="D29" t="n">
+        <v>8.822676E8</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-1.65873E7</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1.06416E8</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1.030493E8</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-3366700.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="n">
+        <v>2.339585E8</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2.35252E8</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1293500.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>